<commit_message>
add ice grid parsing
</commit_message>
<xml_diff>
--- a/dataset/ScheduleTest.xlsx
+++ b/dataset/ScheduleTest.xlsx
@@ -125,13 +125,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -169,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -223,6 +223,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -334,7 +341,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -342,86 +349,86 @@
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -738,13 +745,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="31" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="31" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="32" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="32" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="33" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="33" width="25.862142857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="34" width="29.862142857142857" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="35" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="34" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="32" width="17.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75" customFormat="1" s="1">
@@ -810,7 +817,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33.75">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -831,193 +838,193 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="19"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
@@ -1025,8 +1032,8 @@
       <c r="B26" s="7"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
@@ -1034,8 +1041,8 @@
       <c r="B27" s="7"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
@@ -1043,8 +1050,8 @@
       <c r="B28" s="7"/>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
@@ -1052,8 +1059,8 @@
       <c r="B29" s="7"/>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
@@ -1061,8 +1068,8 @@
       <c r="B30" s="7"/>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
@@ -1070,8 +1077,8 @@
       <c r="B31" s="7"/>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
@@ -1079,8 +1086,8 @@
       <c r="B32" s="7"/>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
@@ -1088,8 +1095,8 @@
       <c r="B33" s="7"/>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
@@ -1097,8 +1104,8 @@
       <c r="B34" s="7"/>
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
@@ -1106,8 +1113,8 @@
       <c r="B35" s="7"/>
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
@@ -1115,8 +1122,8 @@
       <c r="B36" s="7"/>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
@@ -1124,8 +1131,8 @@
       <c r="B37" s="7"/>
       <c r="C37" s="20"/>
       <c r="D37" s="21"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
@@ -1133,8 +1140,8 @@
       <c r="B38" s="7"/>
       <c r="C38" s="20"/>
       <c r="D38" s="21"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
@@ -1142,8 +1149,8 @@
       <c r="B39" s="7"/>
       <c r="C39" s="20"/>
       <c r="D39" s="21"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="23"/>
       <c r="G39" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
@@ -1151,8 +1158,8 @@
       <c r="B40" s="7"/>
       <c r="C40" s="20"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
@@ -1160,8 +1167,8 @@
       <c r="B41" s="7"/>
       <c r="C41" s="20"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
@@ -1169,8 +1176,8 @@
       <c r="B42" s="7"/>
       <c r="C42" s="20"/>
       <c r="D42" s="21"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="23"/>
       <c r="G42" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
@@ -1178,8 +1185,8 @@
       <c r="B43" s="7"/>
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="23"/>
       <c r="G43" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
@@ -1187,8 +1194,8 @@
       <c r="B44" s="7"/>
       <c r="C44" s="20"/>
       <c r="D44" s="21"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
       <c r="G44" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
@@ -1196,23 +1203,23 @@
       <c r="B45" s="7"/>
       <c r="C45" s="20"/>
       <c r="D45" s="21"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="23"/>
       <c r="G45" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D46" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="26" t="s">
+      <c r="F46" s="27" t="s">
         <v>20</v>
       </c>
       <c r="G46" s="7"/>
@@ -1220,16 +1227,16 @@
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
-      <c r="C47" s="27" t="s">
+      <c r="C47" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="28">
+      <c r="D47" s="29">
         <v>22</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="F47" s="31" t="s">
         <v>23</v>
       </c>
       <c r="G47" s="7"/>
@@ -1237,16 +1244,16 @@
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="28">
+      <c r="D48" s="29">
         <v>21</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E48" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="F48" s="31" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="7"/>
@@ -1256,8 +1263,8 @@
       <c r="B49" s="7"/>
       <c r="C49" s="20"/>
       <c r="D49" s="21"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="23"/>
       <c r="G49" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="49.5">
@@ -1267,8 +1274,8 @@
       <c r="B50" s="7"/>
       <c r="C50" s="20"/>
       <c r="D50" s="21"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
       <c r="G50" s="19"/>
     </row>
   </sheetData>

</xml_diff>